<commit_message>
Lecturers can now be parsed including his constrains
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B087DA8-B470-4858-AD66-687E446A6E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4264BA-EAA8-4C28-AD03-C7D62BAF6741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -35,17 +35,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Steven Hawkins</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Albert Einstein</t>
+  </si>
+  <si>
+    <t>Albert Zweistein</t>
+  </si>
+  <si>
+    <t>Konrad Zuse</t>
+  </si>
+  <si>
+    <t>Alan Turing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,12 +101,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -389,20 +432,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAD1A16-556F-4F10-8A98-B67B873665B7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44806</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -410,27 +521,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
fixed issue with lecturer-parser reading the first row
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4264BA-EAA8-4C28-AD03-C7D62BAF6741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2248ED0A-02C3-40CB-8525-890F4E9A2DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added parser function for lectures
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21651355-B8B3-4ADF-94DB-8D202970809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE784C4-D0C7-4912-9EDE-257492BAA7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Steven Hawkins</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
     <t>Albert Zweistein</t>
   </si>
   <si>
@@ -109,12 +106,6 @@
   </si>
   <si>
     <t>Lecturer</t>
-  </si>
-  <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>End Time</t>
   </si>
   <si>
     <t>Holidays</t>
@@ -170,11 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -184,6 +174,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -501,7 +493,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,8 +542,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>44806</v>
@@ -565,7 +557,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -578,7 +570,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>44813</v>
@@ -586,7 +578,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -608,10 +600,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,121 +615,124 @@
     <col min="7" max="7" width="59.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44805</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44861</v>
+      </c>
+      <c r="I3" s="4">
+        <v>44890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5">
-        <v>44805</v>
-      </c>
-      <c r="I2" s="5">
-        <v>44864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5">
-        <v>44861</v>
-      </c>
-      <c r="I3" s="5">
-        <v>44890</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>44896</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>44904</v>
       </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added a group generator with automatic student distribution
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E856FF-98B6-489A-AA32-C3F2FC9128F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8EDB60-1700-4067-B767-F5B41689C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F0E3BE-A749-4FB6-AAB9-11B5EC395D72}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,9 +1012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
generating lectureUnits depending on quantity and groups now working
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8EDB60-1700-4067-B767-F5B41689C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687405AE-D978-4CD6-AA90-9BDFF88865DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
-  <si>
-    <t>Steven Hawkins</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Start Date</t>
   </si>
@@ -81,9 +78,6 @@
     <t>on-site</t>
   </si>
   <si>
-    <t>Georg Mansky-Kummert, Igor Miladinovic, Herbert Paulis</t>
-  </si>
-  <si>
     <t>Exam</t>
   </si>
   <si>
@@ -259,6 +253,9 @@
   </si>
   <si>
     <t>Thor Schuß</t>
+  </si>
+  <si>
+    <t>Georg Mansky-Kummert</t>
   </si>
 </sst>
 </file>
@@ -656,13 +653,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -675,9 +672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,15 +685,15 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>44806</v>
@@ -710,12 +707,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1">
         <v>44814</v>
@@ -723,7 +720,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>44813</v>
@@ -731,7 +728,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -743,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F0E3BE-A749-4FB6-AAB9-11B5EC395D72}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,252 +751,252 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1012,9 +1009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,39 +1024,39 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>4</v>
@@ -1071,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="H2" s="4">
         <v>44805</v>
@@ -1085,10 +1082,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -1100,10 +1097,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H3" s="4">
         <v>44861</v>
@@ -1114,10 +1111,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1129,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4">
         <v>44896</v>

</xml_diff>

<commit_message>
# parser working except general Settings # parser taking multiple lectures # fixed a bug in DayNew.java
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687405AE-D978-4CD6-AA90-9BDFF88865DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4DD9B1-BCED-4A21-99E0-28F309E4E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -24,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>Start Date</t>
   </si>
@@ -256,6 +248,24 @@
   </si>
   <si>
     <t>Georg Mansky-Kummert</t>
+  </si>
+  <si>
+    <t>Georg Mansky-Kummert, Igor Miladinovic, Konrad Zuse</t>
+  </si>
+  <si>
+    <t>Fritz Fischer</t>
+  </si>
+  <si>
+    <t>IT Security ILV</t>
+  </si>
+  <si>
+    <t>Fritz Phantom</t>
+  </si>
+  <si>
+    <t>Albert Zweistein, Alan Turing, Konrad Zuse, Igor Miladinovic, Fritz Phantom</t>
+  </si>
+  <si>
+    <t>Georg Mansky-Kummert, Konrad Zuse</t>
   </si>
 </sst>
 </file>
@@ -308,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -322,7 +332,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -643,7 +652,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,11 +679,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +692,7 @@
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -691,7 +700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -704,13 +713,28 @@
       <c r="D2" s="1">
         <v>44686</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>44809</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44810</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44811</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -718,17 +742,34 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>44813</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44835</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44814</v>
       </c>
     </row>
   </sheetData>
@@ -738,10 +779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F0E3BE-A749-4FB6-AAB9-11B5EC395D72}">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,7 +811,7 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -997,6 +1038,11 @@
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1007,11 +1053,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,10 +1146,10 @@
         <v>12</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H3" s="4">
-        <v>44861</v>
+        <v>44834</v>
       </c>
       <c r="I3" s="4">
         <v>44890</v>
@@ -1132,14 +1178,11 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <v>44896</v>
+        <v>44819</v>
       </c>
       <c r="I4" s="4">
-        <v>44904</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+        <v>44874</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1149,14 +1192,137 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EFF943-C66C-4801-9DF5-CAA9148307CF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="7" max="7" width="75.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44819</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44821</v>
+      </c>
+      <c r="I3" s="4">
+        <v>44890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44805</v>
+      </c>
+      <c r="I4" s="4">
+        <v>44874</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sofar excel has a problem, solve function thourgh out exception.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuhrm\Documents\FH\3.Semester\Software Engineering ILV\Projekt\TimetablePlanner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\IdeaProjects\TimetablePlannerNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BCAE9E-B9E6-4DC4-9B9D-CF5A5C542251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8CBF8-89B7-4573-AD59-E4803BD4F236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,12 @@
     <sheet name="Students" sheetId="6" r:id="rId3"/>
     <sheet name="Software Engineering" sheetId="3" r:id="rId4"/>
     <sheet name="IT Security" sheetId="5" r:id="rId5"/>
+    <sheet name="Datenbank" sheetId="7" r:id="rId6"/>
+    <sheet name="IoT" sheetId="8" r:id="rId7"/>
+    <sheet name="ProjektManagement" sheetId="9" r:id="rId8"/>
+    <sheet name="Mobile App Development" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="164">
   <si>
     <t>Start Date</t>
   </si>
@@ -266,13 +270,268 @@
   </si>
   <si>
     <t>Not Available</t>
+  </si>
+  <si>
+    <t>Samir Brock</t>
+  </si>
+  <si>
+    <t>Levi Rollins</t>
+  </si>
+  <si>
+    <t>Eric Patrick</t>
+  </si>
+  <si>
+    <t>Callum Larson</t>
+  </si>
+  <si>
+    <t>Gabriela Harrington</t>
+  </si>
+  <si>
+    <t>Safiyyah Atkinson</t>
+  </si>
+  <si>
+    <t>Sydney Sandoval</t>
+  </si>
+  <si>
+    <t>Christopher Cummings</t>
+  </si>
+  <si>
+    <t>Clara Steele</t>
+  </si>
+  <si>
+    <t>Dillan Morrison</t>
+  </si>
+  <si>
+    <t>Lottie Goodwin</t>
+  </si>
+  <si>
+    <t>Kieron Bowen</t>
+  </si>
+  <si>
+    <t>Stevie Foley</t>
+  </si>
+  <si>
+    <t>Junaid Kidd</t>
+  </si>
+  <si>
+    <t>Brendon West</t>
+  </si>
+  <si>
+    <t>May Barlow</t>
+  </si>
+  <si>
+    <t>Tomas Hewitt</t>
+  </si>
+  <si>
+    <t>Thalia Randolph</t>
+  </si>
+  <si>
+    <t>Rowan Fischer</t>
+  </si>
+  <si>
+    <t>Tim Turner</t>
+  </si>
+  <si>
+    <t>Syed Mejia</t>
+  </si>
+  <si>
+    <t>Penny Richmond</t>
+  </si>
+  <si>
+    <t>Jeremiah Davenport</t>
+  </si>
+  <si>
+    <t>Katy Ali</t>
+  </si>
+  <si>
+    <t>Keith Keith</t>
+  </si>
+  <si>
+    <t>Cody Archer</t>
+  </si>
+  <si>
+    <t>Annabella Merritt</t>
+  </si>
+  <si>
+    <t>Logan Case</t>
+  </si>
+  <si>
+    <t>Tori Dorsey</t>
+  </si>
+  <si>
+    <t>Chaya Hunter</t>
+  </si>
+  <si>
+    <t>Jennie Wood</t>
+  </si>
+  <si>
+    <t>Ronan Cabrera</t>
+  </si>
+  <si>
+    <t>Tess Mata</t>
+  </si>
+  <si>
+    <t>Rachel Ramsey</t>
+  </si>
+  <si>
+    <t>Musa Simon</t>
+  </si>
+  <si>
+    <t>Kayleigh Fitzpatrick</t>
+  </si>
+  <si>
+    <t>Betty Anthony</t>
+  </si>
+  <si>
+    <t>Kirsten Joyce</t>
+  </si>
+  <si>
+    <t>Roosevelt Hensley</t>
+  </si>
+  <si>
+    <t>Charlie Ward</t>
+  </si>
+  <si>
+    <t>Seth Beasley</t>
+  </si>
+  <si>
+    <t>Nathan Cuevas</t>
+  </si>
+  <si>
+    <t>Cerys Pearce</t>
+  </si>
+  <si>
+    <t>Julius Benton</t>
+  </si>
+  <si>
+    <t>Nieve Summers</t>
+  </si>
+  <si>
+    <t>Nikodem Owen</t>
+  </si>
+  <si>
+    <t>Dhruv Villa</t>
+  </si>
+  <si>
+    <t>Gary Wilson</t>
+  </si>
+  <si>
+    <t>Margaret Arias</t>
+  </si>
+  <si>
+    <t>Ishaan Mueller</t>
+  </si>
+  <si>
+    <t>Manuell Koschuch</t>
+  </si>
+  <si>
+    <t>14/2/2023</t>
+  </si>
+  <si>
+    <t>Lorenz Froihofer</t>
+  </si>
+  <si>
+    <t>16/2/2023</t>
+  </si>
+  <si>
+    <t>29/6/2023</t>
+  </si>
+  <si>
+    <t>Dominik Ertl</t>
+  </si>
+  <si>
+    <t>Karl Michael Göschka</t>
+  </si>
+  <si>
+    <t>30/1/2023</t>
+  </si>
+  <si>
+    <t>13/2/2023</t>
+  </si>
+  <si>
+    <t>Siliva Schmidt</t>
+  </si>
+  <si>
+    <t>28/3/2023</t>
+  </si>
+  <si>
+    <t>Leon Freudenthaler</t>
+  </si>
+  <si>
+    <t>20/2/2023</t>
+  </si>
+  <si>
+    <t>26/6/2023</t>
+  </si>
+  <si>
+    <t>Rene Goldschmidt</t>
+  </si>
+  <si>
+    <t>Thomas Fischer</t>
+  </si>
+  <si>
+    <t>23/5/2023</t>
+  </si>
+  <si>
+    <t>Reinhard Rader</t>
+  </si>
+  <si>
+    <t>Heimo Hirner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernhard Taufner </t>
+  </si>
+  <si>
+    <t>21/2/2023</t>
+  </si>
+  <si>
+    <t>30/6/2023</t>
+  </si>
+  <si>
+    <t>17/3/2023</t>
+  </si>
+  <si>
+    <t>15/5/2023</t>
+  </si>
+  <si>
+    <t>Silvia Schmidt</t>
+  </si>
+  <si>
+    <t>Datenbank</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>ProjektManagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leon Freudenthaler </t>
+  </si>
+  <si>
+    <t>Mobile App Development</t>
+  </si>
+  <si>
+    <t>Heimo Hirner, Silvia Schmidt</t>
+  </si>
+  <si>
+    <t>Karl Michael Göschka, Dominik Ertl</t>
+  </si>
+  <si>
+    <t>Dominik Ertl, Dominik Ertl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leon Freudenthaler, Leon Freudenthaler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rene Schmidt, Rene Schmidt </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +543,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -334,6 +608,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAD1A16-556F-4F10-8A98-B67B873665B7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,6 +966,78 @@
       <c r="B2" s="1">
         <v>44926</v>
       </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45206</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="1">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="1">
+        <v>44987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="1">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="1">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="1">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1">
+        <v>45109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="1">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="1">
+        <v>45171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="1">
+        <v>45201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1">
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1">
+        <v>45262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -687,11 +1047,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,6 +1140,127 @@
         <v>44814</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="10">
+        <v>45206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -788,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F0E3BE-A749-4FB6-AAB9-11B5EC395D72}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,9 +1535,259 @@
         <v>73</v>
       </c>
     </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1064,14 +1795,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
     <col min="5" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="6" width="29.08984375" customWidth="1"/>
     <col min="7" max="7" width="59.6328125" customWidth="1"/>
@@ -1203,16 +1934,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EFF943-C66C-4801-9DF5-CAA9148307CF}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
     <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="29.54296875" customWidth="1"/>
-    <col min="7" max="7" width="75.1796875" customWidth="1"/>
+    <col min="7" max="7" width="63.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1334,4 +2065,570 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B62E189-FE2E-4C04-B781-B3F9B42848C5}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="32.7265625" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44973</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44997</v>
+      </c>
+      <c r="I3" s="4">
+        <v>45061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45099</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A25731-4E5A-4580-8F7C-B16B7C3DAB4F}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44999</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="4">
+        <v>45002</v>
+      </c>
+      <c r="I3" s="4">
+        <v>45071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45096</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA874E9E-852A-41AD-A6E9-3C46E803DBD2}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="12">
+        <v>11</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="13">
+        <v>44971</v>
+      </c>
+      <c r="I2" s="13">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="13">
+        <v>45019</v>
+      </c>
+      <c r="I3" s="13">
+        <v>45052</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="13">
+        <v>45089</v>
+      </c>
+      <c r="I4" s="13">
+        <v>45113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB99504C-744A-4D14-9E2A-764926E634F2}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.36328125" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="12">
+        <v>11</v>
+      </c>
+      <c r="D2" s="12">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="13">
+        <v>44977</v>
+      </c>
+      <c r="I2" s="13">
+        <v>45103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" s="13">
+        <v>44978</v>
+      </c>
+      <c r="I3" s="13">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="13">
+        <v>45101</v>
+      </c>
+      <c r="I4" s="13">
+        <v>45105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All datas in excel are finished correctly but we have still a problem in solve function.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,20 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\IdeaProjects\TimetablePlannerNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8CBF8-89B7-4573-AD59-E4803BD4F236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0785B1-A500-4CBB-BFA8-A91DBCA97827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Lecturers" sheetId="2" r:id="rId2"/>
     <sheet name="Students" sheetId="6" r:id="rId3"/>
-    <sheet name="Software Engineering" sheetId="3" r:id="rId4"/>
-    <sheet name="IT Security" sheetId="5" r:id="rId5"/>
-    <sheet name="Datenbank" sheetId="7" r:id="rId6"/>
-    <sheet name="IoT" sheetId="8" r:id="rId7"/>
-    <sheet name="ProjektManagement" sheetId="9" r:id="rId8"/>
-    <sheet name="Mobile App Development" sheetId="11" r:id="rId9"/>
+    <sheet name="Datenbank" sheetId="7" r:id="rId4"/>
+    <sheet name="IoT" sheetId="8" r:id="rId5"/>
+    <sheet name="ProjektManagement" sheetId="9" r:id="rId6"/>
+    <sheet name="Mobile App Development" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>Start Date</t>
   </si>
@@ -53,9 +51,6 @@
     <t>Alan Turing</t>
   </si>
   <si>
-    <t>Software Engineering ILV</t>
-  </si>
-  <si>
     <t>Lecture</t>
   </si>
   <si>
@@ -251,24 +246,12 @@
     <t>Georg Mansky-Kummert</t>
   </si>
   <si>
-    <t>Georg Mansky-Kummert, Igor Miladinovic, Konrad Zuse</t>
-  </si>
-  <si>
     <t>Fritz Fischer</t>
   </si>
   <si>
-    <t>IT Security ILV</t>
-  </si>
-  <si>
     <t>Fritz Phantom</t>
   </si>
   <si>
-    <t>Albert Zweistein, Alan Turing, Konrad Zuse, Igor Miladinovic, Fritz Phantom</t>
-  </si>
-  <si>
-    <t>Georg Mansky-Kummert, Konrad Zuse</t>
-  </si>
-  <si>
     <t>Not Available</t>
   </si>
   <si>
@@ -425,18 +408,9 @@
     <t>Manuell Koschuch</t>
   </si>
   <si>
-    <t>14/2/2023</t>
-  </si>
-  <si>
     <t>Lorenz Froihofer</t>
   </si>
   <si>
-    <t>16/2/2023</t>
-  </si>
-  <si>
-    <t>29/6/2023</t>
-  </si>
-  <si>
     <t>Dominik Ertl</t>
   </si>
   <si>
@@ -446,33 +420,18 @@
     <t>30/1/2023</t>
   </si>
   <si>
-    <t>13/2/2023</t>
-  </si>
-  <si>
     <t>Siliva Schmidt</t>
   </si>
   <si>
-    <t>28/3/2023</t>
-  </si>
-  <si>
     <t>Leon Freudenthaler</t>
   </si>
   <si>
-    <t>20/2/2023</t>
-  </si>
-  <si>
-    <t>26/6/2023</t>
-  </si>
-  <si>
     <t>Rene Goldschmidt</t>
   </si>
   <si>
     <t>Thomas Fischer</t>
   </si>
   <si>
-    <t>23/5/2023</t>
-  </si>
-  <si>
     <t>Reinhard Rader</t>
   </si>
   <si>
@@ -480,18 +439,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bernhard Taufner </t>
-  </si>
-  <si>
-    <t>21/2/2023</t>
-  </si>
-  <si>
-    <t>30/6/2023</t>
-  </si>
-  <si>
-    <t>17/3/2023</t>
-  </si>
-  <si>
-    <t>15/5/2023</t>
   </si>
   <si>
     <t>Silvia Schmidt</t>
@@ -605,14 +552,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -623,6 +566,8 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,7 +885,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -949,92 +894,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>44805</v>
+      <c r="A2" s="12">
+        <v>44970</v>
       </c>
       <c r="B2" s="1">
-        <v>44926</v>
-      </c>
-      <c r="C2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45206</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44928</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C4" s="1">
-        <v>44959</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C5" s="1">
-        <v>44987</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C6" s="1">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C7" s="1">
-        <v>45048</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="1">
-        <v>45079</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C9" s="1">
-        <v>45109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C10" s="1">
-        <v>45140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C11" s="1">
-        <v>45171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C12" s="1">
-        <v>45201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C13" s="1">
-        <v>45232</v>
+        <v>45117</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C14" s="1">
-        <v>45262</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
@@ -1049,9 +931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F7DCC9-4F44-465E-BF30-CAC24A6588F8}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,12 +947,12 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>44806</v>
@@ -1104,7 +986,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>44814</v>
@@ -1126,7 +1008,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>44835</v>
+        <v>44571</v>
       </c>
       <c r="C6" s="1">
         <v>44814</v>
@@ -1134,7 +1016,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1">
         <v>44814</v>
@@ -1142,10 +1024,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="B8" s="8">
+        <v>44971</v>
       </c>
       <c r="C8" s="1">
         <v>45084</v>
@@ -1153,112 +1035,112 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="B9" s="8">
+        <v>44973</v>
+      </c>
+      <c r="C9" s="8">
+        <v>45106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
+      </c>
+      <c r="B10" s="8">
+        <v>44973</v>
+      </c>
+      <c r="C10" s="8">
+        <v>45106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="B11" s="8">
+        <v>44973</v>
+      </c>
+      <c r="C11" s="8">
+        <v>45106</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="10">
+        <v>129</v>
+      </c>
+      <c r="B12" s="8">
+        <v>45013</v>
+      </c>
+      <c r="C12" s="8">
         <v>45206</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>142</v>
+        <v>130</v>
+      </c>
+      <c r="B13" s="8">
+        <v>44977</v>
+      </c>
+      <c r="C13" s="8">
+        <v>45103</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>142</v>
+        <v>131</v>
+      </c>
+      <c r="B14" s="8">
+        <v>44977</v>
+      </c>
+      <c r="C14" s="8">
+        <v>45103</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>145</v>
+        <v>132</v>
+      </c>
+      <c r="B15" s="8">
+        <v>44971</v>
+      </c>
+      <c r="C15" s="8">
+        <v>45069</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="B16" s="8">
+        <v>44971</v>
+      </c>
+      <c r="C16" s="8">
+        <v>45069</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>150</v>
+        <v>134</v>
+      </c>
+      <c r="B17" s="8">
+        <v>44978</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45107</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>152</v>
+        <v>135</v>
+      </c>
+      <c r="B18" s="8">
+        <v>45002</v>
+      </c>
+      <c r="C18" s="8">
+        <v>45061</v>
       </c>
     </row>
   </sheetData>
@@ -1282,507 +1164,507 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="8" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="8" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="8" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="8" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="8" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="8" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="8" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="8" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="8" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="8" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="8" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="8" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="8" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="8" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="8" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="8" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="8" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="8" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="8" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="8" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="8" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="8" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="8" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="8" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="8" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" s="8" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="8" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" s="8" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="8" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="8" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" s="8" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="8" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" s="8" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" s="8" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" s="8" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="8" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" s="8" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" s="8" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="7" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1792,287 +1674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8AB866-154E-4DEA-A187-603755020D91}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B62E189-FE2E-4C04-B781-B3F9B42848C5}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" customWidth="1"/>
-    <col min="6" max="6" width="29.08984375" customWidth="1"/>
-    <col min="7" max="7" width="59.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4">
-        <v>44805</v>
-      </c>
-      <c r="I2" s="4">
-        <v>44864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="4">
-        <v>44834</v>
-      </c>
-      <c r="I3" s="4">
-        <v>44890</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="4">
-        <v>44819</v>
-      </c>
-      <c r="I4" s="4">
-        <v>44874</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EFF943-C66C-4801-9DF5-CAA9148307CF}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
-    <col min="6" max="6" width="29.54296875" customWidth="1"/>
-    <col min="7" max="7" width="63.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="4">
-        <v>44819</v>
-      </c>
-      <c r="I2" s="4">
-        <v>44895</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="4">
-        <v>44821</v>
-      </c>
-      <c r="I3" s="4">
-        <v>44890</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="4">
-        <v>44805</v>
-      </c>
-      <c r="I4" s="4">
-        <v>44874</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B62E189-FE2E-4C04-B781-B3F9B42848C5}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,25 +1694,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -2117,10 +1723,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>9</v>
@@ -2132,10 +1738,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="H2" s="4">
         <v>44973</v>
@@ -2146,10 +1752,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>6</v>
@@ -2161,24 +1767,24 @@
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H3" s="4">
-        <v>44997</v>
+        <v>44987</v>
       </c>
       <c r="I3" s="4">
-        <v>45061</v>
+        <v>45106</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -2190,16 +1796,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H4" s="4">
         <v>45099</v>
       </c>
       <c r="I4" s="4">
-        <v>45118</v>
+        <v>45106</v>
       </c>
     </row>
   </sheetData>
@@ -2207,12 +1813,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A25731-4E5A-4580-8F7C-B16B7C3DAB4F}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2230,25 +1836,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -2259,10 +1865,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>10</v>
@@ -2274,13 +1880,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="H2" s="4">
-        <v>44999</v>
+        <v>44978</v>
       </c>
       <c r="I2" s="4">
         <v>45107</v>
@@ -2288,10 +1894,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>5</v>
@@ -2303,24 +1909,24 @@
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="H3" s="4">
-        <v>45002</v>
+        <v>44999</v>
       </c>
       <c r="I3" s="4">
-        <v>45071</v>
+        <v>45107</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -2332,16 +1938,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="H4" s="4">
         <v>45096</v>
       </c>
       <c r="I4" s="4">
-        <v>45117</v>
+        <v>45099</v>
       </c>
     </row>
   </sheetData>
@@ -2349,12 +1955,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA874E9E-852A-41AD-A6E9-3C46E803DBD2}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2372,118 +1978,89 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="12">
+      <c r="A2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10">
         <v>11</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>1</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="11">
+        <v>44971</v>
+      </c>
+      <c r="I2" s="11">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="13">
-        <v>44971</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="11">
         <v>45089</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H3" s="13">
-        <v>45019</v>
-      </c>
-      <c r="I3" s="13">
-        <v>45052</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H4" s="13">
-        <v>45089</v>
-      </c>
-      <c r="I4" s="13">
-        <v>45113</v>
+      <c r="I3" s="11">
+        <v>45092</v>
       </c>
     </row>
   </sheetData>
@@ -2492,12 +2069,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB99504C-744A-4D14-9E2A-764926E634F2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2514,117 +2091,117 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10">
+        <v>11</v>
+      </c>
+      <c r="D2" s="10">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="11">
+        <v>44977</v>
+      </c>
+      <c r="I2" s="11">
+        <v>45103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12">
+      <c r="G3" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="11">
+        <v>45055</v>
+      </c>
+      <c r="I3" s="11">
+        <v>45103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12">
-        <v>2</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" s="13">
-        <v>44977</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="11">
         <v>45103</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12">
-        <v>2</v>
-      </c>
-      <c r="E3" s="12">
-        <v>2</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="H3" s="13">
-        <v>44978</v>
-      </c>
-      <c r="I3" s="13">
-        <v>45265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="H4" s="13">
-        <v>45101</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>45105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel has now whole the 4th semester.
All finished !!
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arzbe\IdeaProjects\TimetablePlanner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\IdeaProjects\TimetablePlannerNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8330F58-E996-495C-B7B8-055E90D038F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B940A18E-B384-430F-9481-DE2BE7D80A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{EC82FCA3-5B96-47D8-BD7E-1C3F50D7DE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="IoT" sheetId="8" r:id="rId5"/>
     <sheet name="ProjektManagement" sheetId="9" r:id="rId6"/>
     <sheet name="Mobile App Development" sheetId="11" r:id="rId7"/>
+    <sheet name="Secure Admin Tools" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="143">
   <si>
     <t>Start Date</t>
   </si>
@@ -454,6 +455,12 @@
   </si>
   <si>
     <t>Leon Freudenthaler, Leon Freudenthaler</t>
+  </si>
+  <si>
+    <t>Secure Admin Tools</t>
+  </si>
+  <si>
+    <t>Manuell Koschuch, Silvia Schmidt</t>
   </si>
 </sst>
 </file>
@@ -550,7 +557,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,7 +573,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -868,12 +875,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44970</v>
       </c>
@@ -895,25 +902,25 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="1">
         <v>44624</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="1">
         <v>44625</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="1">
         <v>44626</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
     </row>
   </sheetData>
@@ -928,16 +935,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -945,7 +952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -962,7 +969,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -979,7 +986,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -987,7 +994,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -995,10 +1002,10 @@
         <v>44971</v>
       </c>
       <c r="C5" s="1">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -1009,7 +1016,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1020,7 +1027,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>45117</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>45103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -1064,7 +1071,7 @@
         <v>45103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1075,7 +1082,7 @@
         <v>45069</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -1086,7 +1093,7 @@
         <v>45069</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -1097,7 +1104,7 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -1122,512 +1129,512 @@
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
         <v>120</v>
       </c>
@@ -1643,21 +1650,21 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
-    <col min="7" max="7" width="32.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="32.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1686,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
@@ -1715,7 +1722,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>132</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
@@ -1783,23 +1790,23 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1828,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>133</v>
       </c>
@@ -1857,7 +1864,7 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>133</v>
       </c>
@@ -1886,7 +1893,7 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>133</v>
       </c>
@@ -1928,20 +1935,20 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1970,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>134</v>
       </c>
@@ -1999,7 +2006,7 @@
         <v>45089</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>134</v>
       </c>
@@ -2038,24 +2045,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB99504C-744A-4D14-9E2A-764926E634F2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.453125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -2084,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>135</v>
       </c>
@@ -2113,7 +2120,7 @@
         <v>45103</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>135</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>45103</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>135</v>
       </c>
@@ -2169,6 +2176,118 @@
       </c>
       <c r="I4" s="11">
         <v>45105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1A6BC3-5C60-47C5-BDDA-260FE6538095}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="11">
+        <v>44971</v>
+      </c>
+      <c r="I2" s="11">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="11">
+        <v>44974</v>
+      </c>
+      <c r="I3" s="11">
+        <v>45113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>